<commit_message>
Bug fixes to NWSS feed, notably excluding campus samples and reconfiguring the cvm file.
</commit_message>
<xml_diff>
--- a/patchr/resources/NWSS_map.xlsx
+++ b/patchr/resources/NWSS_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554E9FA7-B7AB-0B47-BE1E-9AB9EB2F0F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A346DA-1804-2A47-B914-D6187EFEDFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="760" windowWidth="29980" windowHeight="14000" xr2:uid="{8B6D7199-4C21-CD4F-9BF8-C2C00BB87A59}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
   <si>
     <t>reporting_jurisdiction</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>NWSS-generated site id; see SOP for new facility partners</t>
+  </si>
+  <si>
+    <t>[translated]</t>
   </si>
 </sst>
 </file>
@@ -442,26 +445,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -781,21 +783,20 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41" style="2" customWidth="1"/>
-    <col min="2" max="3" width="25.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -828,905 +829,907 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4">
+      <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
         <v>2855</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
+      <c r="C16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3" t="s">
+      <c r="C26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4" t="s">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3" t="s">
+      <c r="C28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3" t="s">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3" t="s">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3" t="s">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I34" s="3"/>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="3" t="s">
+      <c r="C35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3" t="s">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3">
+      <c r="C37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2">
         <v>-1</v>
       </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I38" s="3"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="H39" s="3" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="H39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I39" s="3"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="H40" s="3" t="s">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="H40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="3"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3" t="s">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I41" s="3"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="C42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I42" s="3"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="C43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I43" s="3"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="3" t="s">
+      <c r="C44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="3" t="s">
+      <c r="C45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">

</xml_diff>